<commit_message>
or is this not that right kinda fuse
</commit_message>
<xml_diff>
--- a/docs/assets/source_docs/Bill of Materials.xlsx
+++ b/docs/assets/source_docs/Bill of Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\808kb\OneDrive\Documents\GitHub\Tortoise6323\docs\assets\source_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8EAFC1-E793-4C11-A68C-BE05CF7A9DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBFDA30-34CB-4461-A12E-B6E1DD614DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{4B1012BF-1EFD-407A-9053-9C9B9F5468C5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="148">
   <si>
     <t>Unit Quantity</t>
   </si>
@@ -326,9 +326,6 @@
     <t>https://www.keyelco.com/userAssets/file/M65p44.pdf</t>
   </si>
   <si>
-    <t>Peralta 107</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -476,10 +473,13 @@
     <t>P3, P1, P2, J7, J8</t>
   </si>
   <si>
-    <t>Bill Of Materials</t>
-  </si>
-  <si>
     <t>cost</t>
+  </si>
+  <si>
+    <t>Bill of Materials</t>
+  </si>
+  <si>
+    <t>Peralta 109</t>
   </si>
 </sst>
 </file>
@@ -554,7 +554,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -573,57 +573,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -635,14 +629,16 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -982,7 +978,7 @@
   <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:C21"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,1315 +988,1314 @@
     <col min="3" max="6" width="10.7109375" style="4" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" style="3" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" style="3" customWidth="1"/>
-    <col min="9" max="10" width="20.7109375" style="7" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="6" customWidth="1"/>
+    <col min="9" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="5" customWidth="1"/>
     <col min="12" max="12" width="27.7109375" style="3" customWidth="1"/>
     <col min="13" max="13" width="8.7109375" style="2" customWidth="1"/>
     <col min="14" max="14" width="10.7109375" style="2" customWidth="1"/>
     <col min="15" max="16" width="8.7109375" style="2" customWidth="1"/>
     <col min="17" max="17" width="25.7109375" style="3" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="20" t="s">
+      <c r="M3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="20" t="s">
+      <c r="N3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="20" t="s">
+      <c r="O3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="20" t="s">
+      <c r="P3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="20" t="s">
+      <c r="Q3" s="13" t="s">
         <v>16</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B4" s="16">
         <v>1</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="6">
         <v>1.31</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="6">
         <f>B4*C4</f>
         <v>1.31</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="6">
         <v>1.2876000000000001</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="6">
         <f>B4*E4</f>
         <v>1.2876000000000001</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="L4" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="M4" s="13">
+      <c r="M4" s="2">
         <v>2</v>
       </c>
-      <c r="N4" s="14">
+      <c r="N4" s="8">
         <v>45716</v>
       </c>
-      <c r="O4" s="13">
-        <v>0</v>
-      </c>
-      <c r="P4" s="13">
+      <c r="O4" s="2">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2">
         <f>O4-B4</f>
         <v>-1</v>
       </c>
-      <c r="Q4" s="9" t="s">
+      <c r="Q4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="S4" s="24">
+      <c r="S4" s="17">
         <f>M4*C4</f>
         <v>2.62</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B5" s="16">
         <v>1</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="6">
         <v>3.49</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="6">
         <f t="shared" ref="D5:D23" si="0">B5*C5</f>
         <v>3.49</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="6">
         <v>1.98996</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="6">
         <f t="shared" ref="F5:F23" si="1">B5*E5</f>
         <v>1.98996</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="M5" s="13">
+      <c r="M5" s="2">
         <v>2</v>
       </c>
-      <c r="N5" s="14">
+      <c r="N5" s="8">
         <v>45716</v>
       </c>
-      <c r="O5" s="13">
-        <v>0</v>
-      </c>
-      <c r="P5" s="13">
+      <c r="O5" s="2">
+        <v>0</v>
+      </c>
+      <c r="P5" s="2">
         <f t="shared" ref="P5:P23" si="2">O5-B5</f>
         <v>-1</v>
       </c>
-      <c r="Q5" s="9" t="s">
+      <c r="Q5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="S5" s="24">
+      <c r="S5" s="17">
         <f t="shared" ref="S5:S23" si="3">M5*C5</f>
         <v>6.98</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B6" s="16">
         <v>1</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="6">
         <v>6.67</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="6">
         <f t="shared" si="0"/>
         <v>6.67</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="6">
         <v>4.77738</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="6">
         <f t="shared" si="1"/>
         <v>4.77738</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="L6" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="13">
+      <c r="M6" s="2">
         <v>2</v>
       </c>
-      <c r="N6" s="14">
+      <c r="N6" s="8">
         <v>45716</v>
       </c>
-      <c r="O6" s="13">
-        <v>0</v>
-      </c>
-      <c r="P6" s="13">
+      <c r="O6" s="2">
+        <v>0</v>
+      </c>
+      <c r="P6" s="2">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="Q6" s="9" t="s">
+      <c r="Q6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="S6" s="24">
+      <c r="S6" s="17">
         <f t="shared" si="3"/>
         <v>13.34</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B7" s="16">
         <v>1</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="6">
         <v>20.09</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="6">
         <f t="shared" si="0"/>
         <v>20.09</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="6">
         <v>20.09</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="6">
         <f t="shared" si="1"/>
         <v>20.09</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="J7" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="L7" s="16" t="s">
+      <c r="L7" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="M7" s="13">
+      <c r="M7" s="2">
         <v>2</v>
       </c>
-      <c r="N7" s="14">
+      <c r="N7" s="8">
         <v>45716</v>
       </c>
-      <c r="O7" s="13">
-        <v>0</v>
-      </c>
-      <c r="P7" s="13">
+      <c r="O7" s="2">
+        <v>0</v>
+      </c>
+      <c r="P7" s="2">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="Q7" s="9" t="s">
+      <c r="Q7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="S7" s="24">
+      <c r="S7" s="17">
         <f t="shared" si="3"/>
         <v>40.18</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="23">
+      <c r="B8" s="16">
         <v>1</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="6">
         <v>4.54</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="6">
         <f t="shared" si="0"/>
         <v>4.54</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="6">
         <v>1.8202</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="6">
         <f t="shared" si="1"/>
         <v>1.8202</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="K8" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="M8" s="13">
+      <c r="M8" s="2">
         <v>2</v>
       </c>
-      <c r="N8" s="14">
+      <c r="N8" s="8">
         <v>45716</v>
       </c>
-      <c r="O8" s="13">
-        <v>0</v>
-      </c>
-      <c r="P8" s="13">
+      <c r="O8" s="2">
+        <v>0</v>
+      </c>
+      <c r="P8" s="2">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="Q8" s="9" t="s">
+      <c r="Q8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="S8" s="24">
+      <c r="S8" s="17">
         <f t="shared" si="3"/>
         <v>9.08</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="16">
         <v>1</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="6">
         <v>0.39</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="6">
         <f t="shared" si="0"/>
         <v>0.39</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="6">
         <v>0.3</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="6">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="J9" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="L9" s="15" t="s">
+      <c r="L9" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="M9" s="13">
+      <c r="M9" s="2">
         <v>3</v>
       </c>
-      <c r="N9" s="14">
+      <c r="N9" s="8">
         <v>45716</v>
       </c>
-      <c r="O9" s="13">
-        <v>0</v>
-      </c>
-      <c r="P9" s="13">
+      <c r="O9" s="2">
+        <v>0</v>
+      </c>
+      <c r="P9" s="2">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="Q9" s="9" t="s">
+      <c r="Q9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="S9" s="24">
+      <c r="S9" s="17">
         <f t="shared" si="3"/>
         <v>1.17</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="23">
+      <c r="B10" s="16">
         <v>6</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="6">
         <v>0.1</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="6">
         <f t="shared" si="0"/>
         <v>0.60000000000000009</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="6">
         <v>2.4029999999999999E-2</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="6">
         <f t="shared" si="1"/>
         <v>0.14418</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="I10" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="J10" s="11" t="s">
+      <c r="I10" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="K10" s="12" t="s">
+      <c r="J10" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="K10" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="L10" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="M10" s="13">
+      <c r="L10" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="M10" s="2">
         <v>20</v>
       </c>
-      <c r="N10" s="14">
+      <c r="N10" s="8">
         <v>45716</v>
       </c>
-      <c r="O10" s="13">
-        <v>0</v>
-      </c>
-      <c r="P10" s="13">
+      <c r="O10" s="2">
+        <v>0</v>
+      </c>
+      <c r="P10" s="2">
         <f t="shared" si="2"/>
         <v>-6</v>
       </c>
-      <c r="Q10" s="9" t="s">
+      <c r="Q10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="24">
+      <c r="S10" s="17">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="23">
+      <c r="B11" s="16">
         <v>1</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="6">
         <v>0.25</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="6">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="6">
         <v>7.8039999999999998E-2</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="6">
         <f t="shared" si="1"/>
         <v>7.8039999999999998E-2</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="J11" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="I11" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="L11" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="M11" s="13">
+      <c r="L11" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="M11" s="2">
         <v>5</v>
       </c>
-      <c r="N11" s="14">
+      <c r="N11" s="8">
         <v>45716</v>
       </c>
-      <c r="O11" s="13">
-        <v>0</v>
-      </c>
-      <c r="P11" s="13">
+      <c r="O11" s="2">
+        <v>0</v>
+      </c>
+      <c r="P11" s="2">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="Q11" s="9" t="s">
+      <c r="Q11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="S11" s="24">
+      <c r="S11" s="17">
         <f t="shared" si="3"/>
         <v>1.25</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="23">
+      <c r="B12" s="16">
         <v>1</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="6">
         <v>0.15</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="6">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="6">
         <v>4.5659999999999999E-2</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="6">
         <f t="shared" si="1"/>
         <v>4.5659999999999999E-2</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I12" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="K12" s="12" t="s">
+      <c r="I12" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="K12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="L12" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="M12" s="13">
+      <c r="L12" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="M12" s="2">
         <v>5</v>
       </c>
-      <c r="N12" s="14">
+      <c r="N12" s="8">
         <v>45716</v>
       </c>
-      <c r="O12" s="13">
-        <v>0</v>
-      </c>
-      <c r="P12" s="13">
+      <c r="O12" s="2">
+        <v>0</v>
+      </c>
+      <c r="P12" s="2">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="Q12" s="9" t="s">
+      <c r="Q12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="S12" s="24">
+      <c r="S12" s="17">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="23">
+      <c r="B13" s="16">
         <v>1</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="6">
         <v>0.22</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="6">
         <f t="shared" si="0"/>
         <v>0.22</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="6">
         <v>6.7199999999999996E-2</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="6">
         <f t="shared" si="1"/>
         <v>6.7199999999999996E-2</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="H13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="I13" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="J13" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="J13" s="11" t="s">
+      <c r="K13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="L13" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="K13" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="L13" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="M13" s="13">
+      <c r="M13" s="2">
         <v>5</v>
       </c>
-      <c r="N13" s="14">
+      <c r="N13" s="8">
         <v>45716</v>
       </c>
-      <c r="O13" s="13">
-        <v>0</v>
-      </c>
-      <c r="P13" s="13">
+      <c r="O13" s="2">
+        <v>0</v>
+      </c>
+      <c r="P13" s="2">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="Q13" s="9" t="s">
+      <c r="Q13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="S13" s="24">
+      <c r="S13" s="17">
         <f t="shared" si="3"/>
         <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="23">
+      <c r="B14" s="16">
         <v>1</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="6">
         <v>0.25</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="6">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="6">
         <v>7.2059999999999999E-2</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="6">
         <f t="shared" si="1"/>
         <v>7.2059999999999999E-2</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="H14" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I14" s="11" t="s">
+      <c r="I14" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="L14" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="J14" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="L14" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="M14" s="13">
+      <c r="M14" s="2">
         <v>3</v>
       </c>
-      <c r="N14" s="14">
+      <c r="N14" s="8">
         <v>45716</v>
       </c>
-      <c r="O14" s="13">
-        <v>0</v>
-      </c>
-      <c r="P14" s="13">
+      <c r="O14" s="2">
+        <v>0</v>
+      </c>
+      <c r="P14" s="2">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="Q14" s="9" t="s">
+      <c r="Q14" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="S14" s="24">
+      <c r="S14" s="17">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="B15" s="23">
+      <c r="A15" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" s="16">
         <v>1</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="6">
         <v>0.18</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="6">
         <f t="shared" si="0"/>
         <v>0.18</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="6">
         <v>0.1235</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="6">
         <f t="shared" si="1"/>
         <v>0.1235</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="H15" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="J15" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="K15" s="12" t="s">
+      <c r="I15" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="K15" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="L15" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="M15" s="13">
+      <c r="L15" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="M15" s="2">
         <v>3</v>
       </c>
-      <c r="N15" s="14">
+      <c r="N15" s="8">
         <v>45716</v>
       </c>
-      <c r="O15" s="13">
-        <v>0</v>
-      </c>
-      <c r="P15" s="13">
+      <c r="O15" s="2">
+        <v>0</v>
+      </c>
+      <c r="P15" s="2">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="Q15" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="S15" s="24">
+      <c r="Q15" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="S15" s="17">
         <f t="shared" si="3"/>
         <v>0.54</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="B16" s="23">
+      <c r="A16" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" s="16">
         <v>7</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="6">
         <v>0.1</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="6">
         <f t="shared" si="0"/>
         <v>0.70000000000000007</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="6">
         <v>1.0460000000000001E-2</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="6">
         <f t="shared" si="1"/>
         <v>7.3220000000000007E-2</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H16" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="K16" s="12" t="s">
+      <c r="I16" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="K16" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="L16" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="M16" s="13">
+      <c r="L16" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="M16" s="2">
         <v>20</v>
       </c>
-      <c r="N16" s="14">
+      <c r="N16" s="8">
         <v>45716</v>
       </c>
-      <c r="O16" s="13">
-        <v>0</v>
-      </c>
-      <c r="P16" s="13">
+      <c r="O16" s="2">
+        <v>0</v>
+      </c>
+      <c r="P16" s="2">
         <f t="shared" si="2"/>
         <v>-7</v>
       </c>
-      <c r="Q16" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="S16" s="24">
+      <c r="Q16" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="S16" s="17">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="B17" s="23">
+      <c r="A17" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" s="16">
         <v>1</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="6">
         <v>0.11</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="6">
         <f t="shared" si="0"/>
         <v>0.11</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="6">
         <v>1.617E-2</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="6">
         <f t="shared" si="1"/>
         <v>1.617E-2</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="H17" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="J17" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="K17" s="12" t="s">
+      <c r="I17" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="K17" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="L17" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="M17" s="13">
+      <c r="L17" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="M17" s="2">
         <v>5</v>
       </c>
-      <c r="N17" s="14">
+      <c r="N17" s="8">
         <v>45716</v>
       </c>
-      <c r="O17" s="13">
-        <v>0</v>
-      </c>
-      <c r="P17" s="13">
+      <c r="O17" s="2">
+        <v>0</v>
+      </c>
+      <c r="P17" s="2">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="Q17" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="S17" s="24">
+      <c r="Q17" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="S17" s="17">
         <f t="shared" si="3"/>
         <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="23">
+      <c r="B18" s="16">
         <v>1</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="6">
         <v>0.81</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="6">
         <f t="shared" si="0"/>
         <v>0.81</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="6">
         <v>0.36420000000000002</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="6">
         <f t="shared" si="1"/>
         <v>0.36420000000000002</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G18" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="5">
         <v>4628</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="I18" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="J18" s="11" t="s">
+      <c r="J18" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="K18" s="12" t="s">
+      <c r="K18" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="L18" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="L18" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="M18" s="13">
-        <v>0</v>
-      </c>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13">
+      <c r="M18" s="2">
+        <v>0</v>
+      </c>
+      <c r="O18" s="2">
         <v>1</v>
       </c>
-      <c r="P18" s="13">
+      <c r="P18" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q18" s="9" t="s">
+      <c r="Q18" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="S18" s="24">
+      <c r="S18" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="23">
+      <c r="B19" s="16">
         <v>2</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="6">
         <v>0.95</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="6">
         <f t="shared" si="0"/>
         <v>1.9</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="6">
         <v>0.60704999999999998</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="6">
         <f t="shared" si="1"/>
         <v>1.2141</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="H19" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="I19" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="J19" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="J19" s="11" t="s">
+      <c r="K19" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="L19" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="K19" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="L19" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="M19" s="13">
+      <c r="M19" s="2">
         <v>4</v>
       </c>
-      <c r="N19" s="14">
+      <c r="N19" s="8">
         <v>45716</v>
       </c>
-      <c r="O19" s="13">
-        <v>0</v>
-      </c>
-      <c r="P19" s="13">
+      <c r="O19" s="2">
+        <v>0</v>
+      </c>
+      <c r="P19" s="2">
         <f t="shared" si="2"/>
         <v>-2</v>
       </c>
-      <c r="Q19" s="9" t="s">
+      <c r="Q19" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="S19" s="24">
+      <c r="S19" s="17">
         <f t="shared" si="3"/>
         <v>3.8</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B20" s="23">
+      <c r="B20" s="16">
         <v>1</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="6">
         <v>0.17</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="6">
         <f t="shared" si="0"/>
         <v>0.17</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="6">
         <v>0.11156000000000001</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="6">
         <f t="shared" si="1"/>
         <v>0.11156000000000001</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H20" s="9" t="s">
+      <c r="H20" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="I20" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="J20" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="J20" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="K20" s="12" t="s">
+      <c r="K20" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="L20" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="M20" s="13">
+      <c r="L20" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="M20" s="2">
         <v>2</v>
       </c>
-      <c r="N20" s="14">
+      <c r="N20" s="8">
         <v>45716</v>
       </c>
-      <c r="O20" s="13">
-        <v>0</v>
-      </c>
-      <c r="P20" s="13">
+      <c r="O20" s="2">
+        <v>0</v>
+      </c>
+      <c r="P20" s="2">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="Q20" s="9" t="s">
+      <c r="Q20" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="S20" s="24">
+      <c r="S20" s="17">
         <f t="shared" si="3"/>
         <v>0.34</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B21" s="23">
+      <c r="B21" s="16">
         <v>1</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="6">
         <v>0.1</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="6">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="6">
         <v>4.0680000000000001E-2</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="6">
         <f t="shared" si="1"/>
         <v>4.0680000000000001E-2</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="G21" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H21" s="9" t="s">
+      <c r="H21" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="I21" s="11" t="s">
+      <c r="I21" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="L21" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="J21" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="K21" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="L21" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="M21" s="13">
+      <c r="M21" s="2">
         <v>2</v>
       </c>
-      <c r="N21" s="14">
+      <c r="N21" s="8">
         <v>45716</v>
       </c>
-      <c r="O21" s="13">
-        <v>0</v>
-      </c>
-      <c r="P21" s="13">
+      <c r="O21" s="2">
+        <v>0</v>
+      </c>
+      <c r="P21" s="2">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="Q21" s="9" t="s">
+      <c r="Q21" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="S21" s="24">
+      <c r="S21" s="17">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B22" s="23">
+      <c r="B22" s="16">
         <v>1</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="6">
         <v>0.65</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="6">
         <f t="shared" si="0"/>
         <v>0.65</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="6">
         <v>0.41527999999999998</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="6">
         <f t="shared" si="1"/>
         <v>0.41527999999999998</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="G22" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="H22" s="9" t="s">
+      <c r="H22" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="I22" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="J22" s="11" t="s">
+      <c r="I22" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="K22" s="12" t="s">
+      <c r="J22" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="L22" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="L22" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="M22" s="13">
-        <v>0</v>
-      </c>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13">
+      <c r="M22" s="2">
+        <v>0</v>
+      </c>
+      <c r="O22" s="2">
         <v>1</v>
       </c>
-      <c r="P22" s="13">
+      <c r="P22" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q22" s="9" t="s">
+      <c r="Q22" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="S22" s="24">
+      <c r="S22" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B23" s="23">
+      <c r="A23" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" s="16">
         <v>3</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="6">
         <v>0.49</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="6">
         <f t="shared" si="0"/>
         <v>1.47</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="6">
         <v>0.30423</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23" s="6">
         <f t="shared" si="1"/>
         <v>0.91269</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="G23" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="5">
         <v>423751863</v>
       </c>
-      <c r="I23" s="26" t="s">
+      <c r="I23" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="J23" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="J23" s="26" t="s">
+      <c r="K23" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+      <c r="O23" s="2">
+        <v>3</v>
+      </c>
+      <c r="P23" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="K23" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="L23" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="M23" s="13">
-        <v>0</v>
-      </c>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13">
-        <v>3</v>
-      </c>
-      <c r="P23" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q23" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="S23" s="24">
+      <c r="S23" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="T24" s="5">
+      <c r="T24">
         <f>SUM(S:S)</f>
         <v>86.65</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:Q2"/>
+  <mergeCells count="2">
+    <mergeCell ref="I1:Q2"/>
+    <mergeCell ref="A1:H2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I4" r:id="rId1" xr:uid="{116C3F2C-4A84-4F62-A58F-EB1EAF51E578}"/>

</xml_diff>